<commit_message>
Minor updates and testing
</commit_message>
<xml_diff>
--- a/Test output data/Test_Avail_Form.xlsx
+++ b/Test output data/Test_Avail_Form.xlsx
@@ -14,48 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Available</t>
   </si>
-  <si>
-    <t>10/02/2018</t>
-  </si>
-  <si>
-    <t>11/02/2018</t>
-  </si>
-  <si>
-    <t>14/02/2018</t>
-  </si>
-  <si>
-    <t>15/02/2018</t>
-  </si>
-  <si>
-    <t>17/02/2018</t>
-  </si>
-  <si>
-    <t>18/02/2018</t>
-  </si>
-  <si>
-    <t>21/02/2018</t>
-  </si>
-  <si>
-    <t>22/02/2018</t>
-  </si>
-  <si>
-    <t>24/02/2018</t>
-  </si>
-  <si>
-    <t>25/02/2018</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -108,11 +81,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,53 +399,53 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2" s="2">
+        <v>43141</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="2">
+        <v>43142</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" s="2">
+        <v>43145</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="2">
+        <v>43146</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="2">
+        <v>43148</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
+      <c r="A7" s="2">
+        <v>43149</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
+      <c r="A8" s="2">
+        <v>43152</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
+      <c r="A9" s="2">
+        <v>43153</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
+      <c r="A10" s="2">
+        <v>43155</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
+      <c r="A11" s="2">
+        <v>43156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>